<commit_message>
Version 3.1 Sensores de Nivel
</commit_message>
<xml_diff>
--- a/Temperatura_fbr2.xlsx
+++ b/Temperatura_fbr2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20.20725428819662</v>
+        <v>218.9504919815064</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20.18525179147724</v>
+        <v>162.9428252887726</v>
       </c>
     </row>
     <row r="4">
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20.21342386245732</v>
+        <v>210.9375297355652</v>
       </c>
     </row>
     <row r="5">
@@ -469,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20.20540308475495</v>
+        <v>156.9407932186127</v>
       </c>
     </row>
     <row r="6">
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20.20704896688466</v>
+        <v>147.5167701911927</v>
       </c>
     </row>
     <row r="7">
@@ -485,7 +485,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20.19861754655841</v>
+        <v>169.7609234714508</v>
       </c>
     </row>
     <row r="8">
@@ -493,7 +493,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20.18854024410251</v>
+        <v>161.0787859535218</v>
       </c>
     </row>
     <row r="9">
@@ -501,7 +501,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20.14775415897373</v>
+        <v>135.7958772563935</v>
       </c>
     </row>
     <row r="10">
@@ -509,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20.22219969272618</v>
+        <v>191.7397353839875</v>
       </c>
     </row>
     <row r="11">
@@ -517,7 +517,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20.20376051425939</v>
+        <v>165.1139590740204</v>
       </c>
     </row>
     <row r="12">
@@ -525,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20.20780401945115</v>
+        <v>156.382120552063</v>
       </c>
     </row>
     <row r="13">
@@ -533,7 +533,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20.16407058000567</v>
+        <v>157.4156947898865</v>
       </c>
     </row>
     <row r="14">
@@ -541,7 +541,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20.21034073114396</v>
+        <v>171.1493061828613</v>
       </c>
     </row>
     <row r="15">
@@ -549,7 +549,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20.2054726290703</v>
+        <v>171.6427793979645</v>
       </c>
     </row>
     <row r="16">
@@ -557,7 +557,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20.20115425825122</v>
+        <v>179.573070011139</v>
       </c>
     </row>
     <row r="17">
@@ -565,7 +565,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20.18860978841786</v>
+        <v>218.0198698234558</v>
       </c>
     </row>
     <row r="18">
@@ -573,7 +573,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20.2062972259522</v>
+        <v>222.7439555549622</v>
       </c>
     </row>
     <row r="19">
@@ -581,7 +581,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20.21198661327367</v>
+        <v>183.9886836528779</v>
       </c>
     </row>
     <row r="20">
@@ -589,7 +589,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20.20650254726411</v>
+        <v>146.9267032337189</v>
       </c>
     </row>
     <row r="21">
@@ -597,7 +597,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20.20958567857747</v>
+        <v>212.6245820999146</v>
       </c>
     </row>
     <row r="22">
@@ -605,7 +605,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20.20999632120134</v>
+        <v>198.2250938224793</v>
       </c>
     </row>
     <row r="23">
@@ -613,7 +613,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20.18127451896669</v>
+        <v>193.6845123577118</v>
       </c>
     </row>
     <row r="24">
@@ -621,7 +621,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20.21116201639177</v>
+        <v>154.7787862968445</v>
       </c>
     </row>
     <row r="25">
@@ -629,7 +629,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20.21075137376789</v>
+        <v>161.688524017334</v>
       </c>
     </row>
     <row r="26">
@@ -637,7 +637,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20.20410161256791</v>
+        <v>186.6197106838226</v>
       </c>
     </row>
     <row r="27">
@@ -645,7 +645,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20.20656877994543</v>
+        <v>152.8565416812897</v>
       </c>
     </row>
     <row r="28">
@@ -653,7 +653,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20.18175470590597</v>
+        <v>137.8981158065797</v>
       </c>
     </row>
     <row r="29">
@@ -661,7 +661,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20.20986054420473</v>
+        <v>189.1655359935761</v>
       </c>
     </row>
     <row r="30">
@@ -669,7 +669,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20.19855131387715</v>
+        <v>196.4158951473237</v>
       </c>
     </row>
     <row r="31">
@@ -677,7 +677,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20.2093803572655</v>
+        <v>191.5680867671967</v>
       </c>
     </row>
     <row r="32">
@@ -685,7 +685,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20.2093803572655</v>
+        <v>118.1949131107331</v>
       </c>
     </row>
     <row r="33">
@@ -693,7 +693,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20.20670786857607</v>
+        <v>220.319547996521</v>
       </c>
     </row>
     <row r="34">
@@ -701,7 +701,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>20.20800934076311</v>
+        <v>205.1891953277589</v>
       </c>
     </row>
     <row r="35">
@@ -709,7 +709,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20.1969054317475</v>
+        <v>146.0390660858155</v>
       </c>
     </row>
     <row r="36">
@@ -717,7 +717,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20.21082091808324</v>
+        <v>222.883123664856</v>
       </c>
     </row>
     <row r="37">
@@ -725,7 +725,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20.21171174764635</v>
+        <v>213.4426351928711</v>
       </c>
     </row>
     <row r="38">
@@ -733,7 +733,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20.2071880555153</v>
+        <v>147.9150273036958</v>
       </c>
     </row>
     <row r="39">
@@ -741,7 +741,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20.18456628322605</v>
+        <v>206.3845362663269</v>
       </c>
     </row>
     <row r="40">
@@ -749,7 +749,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20.20033297300341</v>
+        <v>206.3006327056885</v>
       </c>
     </row>
     <row r="41">
@@ -757,7 +757,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20.21034073114396</v>
+        <v>153.733621339798</v>
       </c>
     </row>
     <row r="42">
@@ -765,7 +765,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20.19512377262117</v>
+        <v>180.4826434230805</v>
       </c>
     </row>
     <row r="43">
@@ -773,7 +773,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20.21232771158219</v>
+        <v>168.7729305648804</v>
       </c>
     </row>
     <row r="44">
@@ -781,7 +781,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20.19190155267717</v>
+        <v>199.3803374958039</v>
       </c>
     </row>
     <row r="45">
@@ -789,7 +789,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20.19683588743214</v>
+        <v>205.6767208480835</v>
       </c>
     </row>
     <row r="46">
@@ -797,7 +797,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20.1945044970513</v>
+        <v>216.4421808624268</v>
       </c>
     </row>
     <row r="47">
@@ -805,7 +805,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20.20698273420339</v>
+        <v>219.7417340850831</v>
       </c>
     </row>
     <row r="48">
@@ -813,7 +813,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20.20931081295015</v>
+        <v>192.234996881485</v>
       </c>
     </row>
     <row r="49">
@@ -821,7 +821,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20.20087939262396</v>
+        <v>194.1080041217804</v>
       </c>
     </row>
     <row r="50">
@@ -829,7 +829,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20.18723877191547</v>
+        <v>219.017254524231</v>
       </c>
     </row>
     <row r="51">
@@ -837,7 +837,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20.20574749469762</v>
+        <v>186.5459539699555</v>
       </c>
     </row>
     <row r="52">
@@ -845,7 +845,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20.20924458026889</v>
+        <v>169.7810714530945</v>
       </c>
     </row>
     <row r="53">
@@ -853,7 +853,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20.19464358568194</v>
+        <v>237.4104410171509</v>
       </c>
     </row>
     <row r="54">
@@ -861,7 +861,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>20.20451225519184</v>
+        <v>226.1460899543763</v>
       </c>
     </row>
     <row r="55">
@@ -869,7 +869,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>20.20848952770234</v>
+        <v>144.3581203746796</v>
       </c>
     </row>
     <row r="56">
@@ -877,7 +877,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>20.20485666513446</v>
+        <v>118.5343688488007</v>
       </c>
     </row>
     <row r="57">
@@ -885,7 +885,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>20.1861426210404</v>
+        <v>199.3860997390748</v>
       </c>
     </row>
     <row r="58">
@@ -893,7 +893,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>20.20362142562868</v>
+        <v>149.0802191257477</v>
       </c>
     </row>
     <row r="59">
@@ -901,7 +901,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>20.21410937070851</v>
+        <v>141.7160589790345</v>
       </c>
     </row>
     <row r="60">
@@ -909,7 +909,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>20.22343162059786</v>
+        <v>144.6504184436799</v>
       </c>
     </row>
     <row r="61">
@@ -917,7 +917,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>20.20643300294881</v>
+        <v>143.0428188037873</v>
       </c>
     </row>
     <row r="62">
@@ -925,7 +925,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>20.21177798032761</v>
+        <v>209.1268342018128</v>
       </c>
     </row>
     <row r="63">
@@ -933,7 +933,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>20.20581703901291</v>
+        <v>185.3883789062501</v>
       </c>
     </row>
     <row r="64">
@@ -941,7 +941,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>20.20828420639043</v>
+        <v>183.3768261432648</v>
       </c>
     </row>
     <row r="65">
@@ -949,7 +949,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>20.18675858497625</v>
+        <v>156.2031466007233</v>
       </c>
     </row>
     <row r="66">
@@ -957,7 +957,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>20.16496140956883</v>
+        <v>234.1883800315857</v>
       </c>
     </row>
     <row r="67">
@@ -965,7 +965,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>20.21136733770373</v>
+        <v>186.519010515213</v>
       </c>
     </row>
     <row r="68">
@@ -973,7 +973,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>20.18812960147864</v>
+        <v>167.0206257629395</v>
       </c>
     </row>
     <row r="69">
@@ -981,7 +981,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>20.19724653005602</v>
+        <v>128.9151362037659</v>
       </c>
     </row>
     <row r="70">
@@ -989,7 +989,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>20.19855131387715</v>
+        <v>176.5374142837525</v>
       </c>
     </row>
     <row r="71">
@@ -997,7 +997,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>20.20711851119995</v>
+        <v>173.4187292671204</v>
       </c>
     </row>
     <row r="72">
@@ -1005,7 +1005,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>20.16982951164249</v>
+        <v>170.3716815185547</v>
       </c>
     </row>
     <row r="73">
@@ -1013,7 +1013,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>20.20841998338705</v>
+        <v>107.6412784576416</v>
       </c>
     </row>
     <row r="74">
@@ -1021,7 +1021,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>20.21150642633438</v>
+        <v>208.8461136054993</v>
       </c>
     </row>
     <row r="75">
@@ -1029,7 +1029,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>20.20896971464163</v>
+        <v>155.1084263515473</v>
       </c>
     </row>
     <row r="76">
@@ -1037,7 +1037,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>20.19327256917956</v>
+        <v>184.2105101490021</v>
       </c>
     </row>
     <row r="77">
@@ -1045,7 +1045,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>20.23474416255954</v>
+        <v>150.6782812595368</v>
       </c>
     </row>
     <row r="78">
@@ -1053,7 +1053,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>20.18593729972844</v>
+        <v>173.3951504325867</v>
       </c>
     </row>
     <row r="79">
@@ -1061,7 +1061,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>20.19649478912356</v>
+        <v>173.9964636993409</v>
       </c>
     </row>
     <row r="80">
@@ -1069,7 +1069,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>20.2054726290703</v>
+        <v>165.6525367450714</v>
       </c>
     </row>
     <row r="81">
@@ -1077,7 +1077,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>20.21075137376789</v>
+        <v>158.5893908882142</v>
       </c>
     </row>
     <row r="82">
@@ -1085,7 +1085,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>20.18401655197147</v>
+        <v>180.2994173336029</v>
       </c>
     </row>
     <row r="83">
@@ -1093,7 +1093,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>20.21472864627839</v>
+        <v>197.1385996723176</v>
       </c>
     </row>
     <row r="84">
@@ -1101,7 +1101,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>20.20451225519184</v>
+        <v>148.9178298377991</v>
       </c>
     </row>
     <row r="85">
@@ -1109,7 +1109,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>20.20135957956319</v>
+        <v>159.6959667873383</v>
       </c>
     </row>
     <row r="86">
@@ -1117,7 +1117,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>20.21458955764774</v>
+        <v>187.5396296405793</v>
       </c>
     </row>
     <row r="87">
@@ -1125,7 +1125,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>20.21815618753436</v>
+        <v>207.328855342865</v>
       </c>
     </row>
     <row r="88">
@@ -1133,7 +1133,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>20.17880735158923</v>
+        <v>173.6854482746124</v>
       </c>
     </row>
     <row r="89">
@@ -1141,7 +1141,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>20.15282758235935</v>
+        <v>167.8326516819001</v>
       </c>
     </row>
     <row r="90">
@@ -1149,7 +1149,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>20.21075137376789</v>
+        <v>182.7627034759522</v>
       </c>
     </row>
     <row r="91">
@@ -1157,7 +1157,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>20.1953953266144</v>
+        <v>169.1217780971527</v>
       </c>
     </row>
     <row r="92">
@@ -1165,7 +1165,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>20.21500020027162</v>
+        <v>202.316193819046</v>
       </c>
     </row>
     <row r="93">
@@ -1173,7 +1173,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>20.21561947584155</v>
+        <v>171.9082664775849</v>
       </c>
     </row>
     <row r="94">
@@ -1181,7 +1181,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>20.22068958759309</v>
+        <v>213.530512714386</v>
       </c>
     </row>
     <row r="95">
@@ -1189,7 +1189,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>20.19375275611878</v>
+        <v>198.226325750351</v>
       </c>
     </row>
     <row r="96">
@@ -1197,7 +1197,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>20.130619764328</v>
+        <v>181.8717811870575</v>
       </c>
     </row>
     <row r="97">
@@ -1205,7 +1205,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>20.20273059606552</v>
+        <v>222.7012487220765</v>
       </c>
     </row>
     <row r="98">
@@ -1213,7 +1213,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>20.21699049234394</v>
+        <v>197.3377348518372</v>
       </c>
     </row>
     <row r="99">
@@ -1221,7 +1221,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>20.18751363754274</v>
+        <v>215.1444706916809</v>
       </c>
     </row>
     <row r="100">
@@ -1229,7 +1229,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>20.21191706895831</v>
+        <v>114.2310328483582</v>
       </c>
     </row>
     <row r="101">
@@ -1237,7 +1237,527 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>20.21177798032761</v>
+        <v>211.90672580719</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="n">
+        <v>166.3111545276643</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="n">
+        <v>157.6827582073212</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="n">
+        <v>208.5590346717835</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="n">
+        <v>202.541795578003</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>172.0227430438996</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="n">
+        <v>157.5648640346527</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="n">
+        <v>195.1310208702088</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="n">
+        <v>218.8415789604187</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>190.9199602413178</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>167.9628916263581</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>160.3895289325715</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="n">
+        <v>161.2865578746796</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="n">
+        <v>172.0795044517517</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="n">
+        <v>223.3589127540589</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="n">
+        <v>217.8159526443482</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="n">
+        <v>176.1856260204315</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="n">
+        <v>165.734731502533</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="n">
+        <v>193.0920477771759</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="n">
+        <v>191.0120236682892</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="n">
+        <v>160.5366449642182</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="n">
+        <v>165.4354525089265</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="n">
+        <v>172.0160270500184</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="n">
+        <v>111.9043052482605</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>182.9178998947144</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="n">
+        <v>198.4857194232941</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="n">
+        <v>165.8505724620819</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>164.0816167640686</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="n">
+        <v>183.431044216156</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="n">
+        <v>178.3703242588043</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="n">
+        <v>166.8244445610047</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="n">
+        <v>233.7849170303345</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="n">
+        <v>200.437901210785</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="n">
+        <v>166.2358214759827</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="n">
+        <v>200.8662677001954</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="n">
+        <v>211.3945352363587</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="n">
+        <v>205.8576155471802</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="n">
+        <v>176.3785883140564</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="n">
+        <v>218.7188100624085</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="n">
+        <v>217.278196258545</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="n">
+        <v>146.4260239028931</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="n">
+        <v>182.876769399643</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="n">
+        <v>198.1434554195404</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="n">
+        <v>180.6501061344147</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>172.3198363590241</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="n">
+        <v>186.027047405243</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="n">
+        <v>214.1142080879212</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="n">
+        <v>227.2311932182312</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="n">
+        <v>249.8055694007875</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>191.4335284519196</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>176.8794663429261</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="n">
+        <v>180.235184879303</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="n">
+        <v>216.8981531333924</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="n">
+        <v>190.3138517284394</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="n">
+        <v>145.8859228801728</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="n">
+        <v>230.5218712615967</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="n">
+        <v>207.9059804344178</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="n">
+        <v>161.1435615158081</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="n">
+        <v>198.9178479290009</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="n">
+        <v>204.0207845973969</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="n">
+        <v>199.5044840335846</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="n">
+        <v>175.8991564273834</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="n">
+        <v>169.0430141925812</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>194.6130018234253</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>144.1894919681549</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="n">
+        <v>224.3374343872071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>